<commit_message>
fixing up permissions and errorhandling
</commit_message>
<xml_diff>
--- a/differences_output.xlsx
+++ b/differences_output.xlsx
@@ -2134,7 +2134,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2142,7 +2142,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2158,7 +2158,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>-0.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2182,7 +2182,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>-0.02999999999999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2206,7 +2206,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2214,7 +2214,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0.01999999999999996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -2326,7 +2326,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>-0.23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -2342,7 +2342,7 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>0.06999999999999984</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -2358,7 +2358,7 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -2374,7 +2374,7 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>-0.04000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -2389,6 +2389,9 @@
       <c r="A35" t="s">
         <v>35</v>
       </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
@@ -2403,7 +2406,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>-0.0900000000000003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -2411,7 +2414,7 @@
         <v>38</v>
       </c>
       <c r="B38">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -2435,7 +2438,7 @@
         <v>41</v>
       </c>
       <c r="B41">
-        <v>-0.009999999999999995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -2443,7 +2446,7 @@
         <v>42</v>
       </c>
       <c r="B42">
-        <v>0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -2459,7 +2462,7 @@
         <v>44</v>
       </c>
       <c r="B44">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -2467,7 +2470,7 @@
         <v>45</v>
       </c>
       <c r="B45">
-        <v>-0.009999999999999953</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -2507,7 +2510,7 @@
         <v>50</v>
       </c>
       <c r="B50">
-        <v>-0.02000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -2539,7 +2542,7 @@
         <v>54</v>
       </c>
       <c r="B54">
-        <v>-0.009999999999999995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -2547,7 +2550,7 @@
         <v>55</v>
       </c>
       <c r="B55">
-        <v>0.0199999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -2555,7 +2558,7 @@
         <v>56</v>
       </c>
       <c r="B56">
-        <v>-0.06999999999999984</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -2563,7 +2566,7 @@
         <v>57</v>
       </c>
       <c r="B57">
-        <v>0.009999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -2579,7 +2582,7 @@
         <v>59</v>
       </c>
       <c r="B59">
-        <v>0.009999999999999981</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -2587,20 +2590,23 @@
         <v>60</v>
       </c>
       <c r="B60">
-        <v>-0.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
         <v>61</v>
       </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
         <v>62</v>
       </c>
       <c r="B62">
-        <v>-0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -2608,7 +2614,7 @@
         <v>63</v>
       </c>
       <c r="B63">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -2616,7 +2622,7 @@
         <v>64</v>
       </c>
       <c r="B64">
-        <v>0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -2624,7 +2630,7 @@
         <v>65</v>
       </c>
       <c r="B65">
-        <v>0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -2656,7 +2662,7 @@
         <v>69</v>
       </c>
       <c r="B69">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -2672,7 +2678,7 @@
         <v>71</v>
       </c>
       <c r="B71">
-        <v>0.009999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -2688,7 +2694,7 @@
         <v>73</v>
       </c>
       <c r="B73">
-        <v>-0.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -2704,7 +2710,7 @@
         <v>75</v>
       </c>
       <c r="B75">
-        <v>-0.1699999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -2712,7 +2718,7 @@
         <v>76</v>
       </c>
       <c r="B76">
-        <v>-0.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -2728,7 +2734,7 @@
         <v>78</v>
       </c>
       <c r="B78">
-        <v>-0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -2736,7 +2742,7 @@
         <v>79</v>
       </c>
       <c r="B79">
-        <v>0.009999999999999995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -2752,7 +2758,7 @@
         <v>81</v>
       </c>
       <c r="B81">
-        <v>-0.02000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -2816,7 +2822,7 @@
         <v>89</v>
       </c>
       <c r="B89">
-        <v>-0.009999999999999988</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -2831,6 +2837,9 @@
       <c r="A91" t="s">
         <v>91</v>
       </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
@@ -2853,7 +2862,7 @@
         <v>94</v>
       </c>
       <c r="B94">
-        <v>-0.04000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -2861,7 +2870,7 @@
         <v>95</v>
       </c>
       <c r="B95">
-        <v>0.04000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -2884,13 +2893,16 @@
       <c r="A98" t="s">
         <v>98</v>
       </c>
+      <c r="B98">
+        <v>0</v>
+      </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
         <v>99</v>
       </c>
       <c r="B99">
-        <v>0.0199999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -2914,7 +2926,7 @@
         <v>102</v>
       </c>
       <c r="B102">
-        <v>0.009999999999999995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -2945,13 +2957,16 @@
       <c r="A106" t="s">
         <v>106</v>
       </c>
+      <c r="B106">
+        <v>0</v>
+      </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
         <v>107</v>
       </c>
       <c r="B107">
-        <v>-0.01000000000000006</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -2967,7 +2982,7 @@
         <v>109</v>
       </c>
       <c r="B109">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -2999,7 +3014,7 @@
         <v>113</v>
       </c>
       <c r="B113">
-        <v>-0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -3023,7 +3038,7 @@
         <v>116</v>
       </c>
       <c r="B116">
-        <v>0.009999999999999981</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -3031,7 +3046,7 @@
         <v>117</v>
       </c>
       <c r="B117">
-        <v>0.01999999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -3055,7 +3070,7 @@
         <v>120</v>
       </c>
       <c r="B120">
-        <v>0.009999999999999787</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -3127,7 +3142,7 @@
         <v>129</v>
       </c>
       <c r="B129">
-        <v>-0.02000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -3143,7 +3158,7 @@
         <v>131</v>
       </c>
       <c r="B131">
-        <v>0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -3159,7 +3174,7 @@
         <v>133</v>
       </c>
       <c r="B133">
-        <v>-0.009999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -3175,7 +3190,7 @@
         <v>135</v>
       </c>
       <c r="B135">
-        <v>0.009999999999999995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -3190,6 +3205,9 @@
       <c r="A137" t="s">
         <v>137</v>
       </c>
+      <c r="B137">
+        <v>0</v>
+      </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
@@ -3228,7 +3246,7 @@
         <v>142</v>
       </c>
       <c r="B142">
-        <v>-0.05000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -3236,7 +3254,7 @@
         <v>143</v>
       </c>
       <c r="B143">
-        <v>-0.03999999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -3252,7 +3270,7 @@
         <v>145</v>
       </c>
       <c r="B145">
-        <v>-0.1699999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -3268,7 +3286,7 @@
         <v>147</v>
       </c>
       <c r="B147">
-        <v>0.05000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -3283,13 +3301,16 @@
       <c r="A149" t="s">
         <v>149</v>
       </c>
+      <c r="B149">
+        <v>0</v>
+      </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
         <v>150</v>
       </c>
       <c r="B150">
-        <v>0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -3305,7 +3326,7 @@
         <v>152</v>
       </c>
       <c r="B152">
-        <v>0.1099999999999977</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -3353,7 +3374,7 @@
         <v>158</v>
       </c>
       <c r="B158">
-        <v>0.009999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -3361,7 +3382,7 @@
         <v>159</v>
       </c>
       <c r="B159">
-        <v>0.04999999999999993</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -3369,7 +3390,7 @@
         <v>160</v>
       </c>
       <c r="B160">
-        <v>0.02000000000000046</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -3377,7 +3398,7 @@
         <v>161</v>
       </c>
       <c r="B161">
-        <v>-0.02999999999999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -3408,13 +3429,16 @@
       <c r="A165" t="s">
         <v>165</v>
       </c>
+      <c r="B165">
+        <v>0</v>
+      </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" t="s">
         <v>166</v>
       </c>
       <c r="B166">
-        <v>0.03000000000000003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -3438,7 +3462,7 @@
         <v>169</v>
       </c>
       <c r="B169">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -3461,6 +3485,9 @@
       <c r="A172" t="s">
         <v>172</v>
       </c>
+      <c r="B172">
+        <v>0</v>
+      </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" t="s">
@@ -3483,20 +3510,23 @@
         <v>175</v>
       </c>
       <c r="B175">
-        <v>-4.440892098500626E-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" t="s">
         <v>176</v>
       </c>
+      <c r="B176">
+        <v>0</v>
+      </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" t="s">
         <v>177</v>
       </c>
       <c r="B177">
-        <v>0.009999999999999995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="178" spans="1:2">
@@ -3528,7 +3558,7 @@
         <v>181</v>
       </c>
       <c r="B181">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -3544,7 +3574,7 @@
         <v>183</v>
       </c>
       <c r="B183">
-        <v>-0.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -3568,7 +3598,7 @@
         <v>186</v>
       </c>
       <c r="B186">
-        <v>-0.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="187" spans="1:2">
@@ -3600,7 +3630,7 @@
         <v>190</v>
       </c>
       <c r="B190">
-        <v>0.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="191" spans="1:2">
@@ -3656,7 +3686,7 @@
         <v>197</v>
       </c>
       <c r="B197">
-        <v>0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -3688,7 +3718,7 @@
         <v>201</v>
       </c>
       <c r="B201">
-        <v>0.02000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -3720,7 +3750,7 @@
         <v>205</v>
       </c>
       <c r="B205">
-        <v>0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="206" spans="1:2">
@@ -3752,20 +3782,23 @@
         <v>209</v>
       </c>
       <c r="B209">
-        <v>0.01999999999999996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="210" spans="1:2">
       <c r="A210" t="s">
         <v>210</v>
       </c>
+      <c r="B210">
+        <v>0</v>
+      </c>
     </row>
     <row r="211" spans="1:2">
       <c r="A211" t="s">
         <v>211</v>
       </c>
       <c r="B211">
-        <v>0.6299999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -3781,7 +3814,7 @@
         <v>213</v>
       </c>
       <c r="B213">
-        <v>0.1099999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="214" spans="1:2">
@@ -3789,7 +3822,7 @@
         <v>214</v>
       </c>
       <c r="B214">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="215" spans="1:2">
@@ -3797,7 +3830,7 @@
         <v>215</v>
       </c>
       <c r="B215">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="216" spans="1:2">
@@ -3805,7 +3838,7 @@
         <v>216</v>
       </c>
       <c r="B216">
-        <v>0.03999999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="217" spans="1:2">
@@ -3821,7 +3854,7 @@
         <v>218</v>
       </c>
       <c r="B218">
-        <v>0.009999999999999995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="219" spans="1:2">
@@ -3837,7 +3870,7 @@
         <v>220</v>
       </c>
       <c r="B220">
-        <v>0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="221" spans="1:2">
@@ -3845,7 +3878,7 @@
         <v>221</v>
       </c>
       <c r="B221">
-        <v>-0.4499999999999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="222" spans="1:2">
@@ -3853,7 +3886,7 @@
         <v>222</v>
       </c>
       <c r="B222">
-        <v>0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="223" spans="1:2">
@@ -3909,7 +3942,7 @@
         <v>229</v>
       </c>
       <c r="B229">
-        <v>0.09</v>
+        <v>0</v>
       </c>
     </row>
     <row r="230" spans="1:2">
@@ -3917,7 +3950,7 @@
         <v>230</v>
       </c>
       <c r="B230">
-        <v>0.1199999999999992</v>
+        <v>0</v>
       </c>
     </row>
     <row r="231" spans="1:2">
@@ -3925,7 +3958,7 @@
         <v>231</v>
       </c>
       <c r="B231">
-        <v>-0.009999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="232" spans="1:2">
@@ -3965,7 +3998,7 @@
         <v>236</v>
       </c>
       <c r="B236">
-        <v>0.02000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="237" spans="1:2">
@@ -4018,7 +4051,7 @@
         <v>240</v>
       </c>
       <c r="B2">
-        <v>0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4034,7 +4067,7 @@
         <v>242</v>
       </c>
       <c r="B4">
-        <v>0.04999999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4042,7 +4075,7 @@
         <v>243</v>
       </c>
       <c r="B5">
-        <v>-0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4114,7 +4147,7 @@
         <v>252</v>
       </c>
       <c r="B14">
-        <v>0.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -4138,7 +4171,7 @@
         <v>255</v>
       </c>
       <c r="B17">
-        <v>0.009999999999999995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -4162,7 +4195,7 @@
         <v>258</v>
       </c>
       <c r="B20">
-        <v>-0.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -4186,7 +4219,7 @@
         <v>261</v>
       </c>
       <c r="B23">
-        <v>-0.0900000000000003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -4202,7 +4235,7 @@
         <v>263</v>
       </c>
       <c r="B25">
-        <v>0.07000000000000028</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -4218,7 +4251,7 @@
         <v>265</v>
       </c>
       <c r="B27">
-        <v>-0.009999999999999787</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -4226,7 +4259,7 @@
         <v>266</v>
       </c>
       <c r="B28">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -4242,7 +4275,7 @@
         <v>268</v>
       </c>
       <c r="B30">
-        <v>-0.02000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -4250,7 +4283,7 @@
         <v>269</v>
       </c>
       <c r="B31">
-        <v>0.009999999999999981</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -4258,7 +4291,7 @@
         <v>270</v>
       </c>
       <c r="B32">
-        <v>-0.009999999999999787</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -4266,7 +4299,7 @@
         <v>74</v>
       </c>
       <c r="B33">
-        <v>0.0199999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -4290,7 +4323,7 @@
         <v>273</v>
       </c>
       <c r="B36">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -4298,7 +4331,7 @@
         <v>274</v>
       </c>
       <c r="B37">
-        <v>-0.1299999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -4306,7 +4339,7 @@
         <v>91</v>
       </c>
       <c r="B38">
-        <v>0.01999999999999996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -4314,7 +4347,7 @@
         <v>275</v>
       </c>
       <c r="B39">
-        <v>-0.1600000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -4362,7 +4395,7 @@
         <v>281</v>
       </c>
       <c r="B45">
-        <v>-0.05000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -4386,7 +4419,7 @@
         <v>284</v>
       </c>
       <c r="B48">
-        <v>-0.01999999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -4402,7 +4435,7 @@
         <v>286</v>
       </c>
       <c r="B50">
-        <v>-0.09999999999999964</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -4410,7 +4443,7 @@
         <v>152</v>
       </c>
       <c r="B51">
-        <v>0.05999999999999872</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -4418,7 +4451,7 @@
         <v>287</v>
       </c>
       <c r="B52">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -4426,7 +4459,7 @@
         <v>288</v>
       </c>
       <c r="B53">
-        <v>0.02999999999999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -4434,7 +4467,7 @@
         <v>289</v>
       </c>
       <c r="B54">
-        <v>0.01999999999999996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -4442,7 +4475,7 @@
         <v>154</v>
       </c>
       <c r="B55">
-        <v>-0.4300000000000015</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -4490,7 +4523,7 @@
         <v>295</v>
       </c>
       <c r="B61">
-        <v>0.02000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -4506,7 +4539,7 @@
         <v>297</v>
       </c>
       <c r="B63">
-        <v>-0.02000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -4522,7 +4555,7 @@
         <v>299</v>
       </c>
       <c r="B65">
-        <v>-0.1300000000000003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -4530,7 +4563,7 @@
         <v>300</v>
       </c>
       <c r="B66">
-        <v>-0.009999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -4538,7 +4571,7 @@
         <v>301</v>
       </c>
       <c r="B67">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -4546,7 +4579,7 @@
         <v>302</v>
       </c>
       <c r="B68">
-        <v>-0.02999999999999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -4570,7 +4603,7 @@
         <v>305</v>
       </c>
       <c r="B71">
-        <v>0.02000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -4602,7 +4635,7 @@
         <v>308</v>
       </c>
       <c r="B75">
-        <v>0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -4610,7 +4643,7 @@
         <v>309</v>
       </c>
       <c r="B76">
-        <v>-0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -4626,7 +4659,7 @@
         <v>310</v>
       </c>
       <c r="B78">
-        <v>6.92</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -4658,7 +4691,7 @@
         <v>314</v>
       </c>
       <c r="B82">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -4703,7 +4736,7 @@
         <v>316</v>
       </c>
       <c r="B2">
-        <v>-0.08000000000000185</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4711,7 +4744,7 @@
         <v>317</v>
       </c>
       <c r="B3">
-        <v>0.07999999999999829</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4764,7 +4797,7 @@
         <v>321</v>
       </c>
       <c r="B5">
-        <v>0.04000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4788,7 +4821,7 @@
         <v>324</v>
       </c>
       <c r="B8">
-        <v>0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4796,7 +4829,7 @@
         <v>325</v>
       </c>
       <c r="B9">
-        <v>0.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4812,7 +4845,7 @@
         <v>327</v>
       </c>
       <c r="B11">
-        <v>-0.1399999999999988</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -4820,7 +4853,7 @@
         <v>328</v>
       </c>
       <c r="B12">
-        <v>-0.05999999999999961</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -4828,7 +4861,7 @@
         <v>329</v>
       </c>
       <c r="B13">
-        <v>0.05000000000000071</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -4844,7 +4877,7 @@
         <v>331</v>
       </c>
       <c r="B15">
-        <v>0.03000000000000003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -4908,7 +4941,7 @@
         <v>339</v>
       </c>
       <c r="B23">
-        <v>-0.06</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -4916,7 +4949,7 @@
         <v>340</v>
       </c>
       <c r="B24">
-        <v>-0.02000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -4939,6 +4972,9 @@
       <c r="A27" t="s">
         <v>343</v>
       </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
@@ -4985,7 +5021,7 @@
         <v>349</v>
       </c>
       <c r="B33">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -5001,7 +5037,7 @@
         <v>351</v>
       </c>
       <c r="B35">
-        <v>-0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -5009,7 +5045,7 @@
         <v>352</v>
       </c>
       <c r="B36">
-        <v>-0.01999999999999991</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -5017,7 +5053,7 @@
         <v>353</v>
       </c>
       <c r="B37">
-        <v>-0.009999999999999898</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -5025,7 +5061,7 @@
         <v>354</v>
       </c>
       <c r="B38">
-        <v>-0.009999999999999953</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -5073,7 +5109,7 @@
         <v>360</v>
       </c>
       <c r="B44">
-        <v>0.05000000000000071</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -5081,7 +5117,7 @@
         <v>361</v>
       </c>
       <c r="B45">
-        <v>0.02000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -5105,7 +5141,7 @@
         <v>364</v>
       </c>
       <c r="B48">
-        <v>-0.009999999999999343</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -5161,7 +5197,7 @@
         <v>371</v>
       </c>
       <c r="B55">
-        <v>-0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -5177,7 +5213,7 @@
         <v>373</v>
       </c>
       <c r="B57">
-        <v>0.01000000000000068</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -5193,7 +5229,7 @@
         <v>375</v>
       </c>
       <c r="B59">
-        <v>0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -5201,7 +5237,7 @@
         <v>376</v>
       </c>
       <c r="B60">
-        <v>0.02000000000000013</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -5209,7 +5245,7 @@
         <v>377</v>
       </c>
       <c r="B61">
-        <v>0.009999999999999898</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -5217,7 +5253,7 @@
         <v>378</v>
       </c>
       <c r="B62">
-        <v>0.03999999999999915</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -5225,7 +5261,7 @@
         <v>379</v>
       </c>
       <c r="B63">
-        <v>-0.01000000000000023</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -5233,7 +5269,7 @@
         <v>380</v>
       </c>
       <c r="B64">
-        <v>-0.1199999999999992</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -5249,7 +5285,7 @@
         <v>382</v>
       </c>
       <c r="B66">
-        <v>0.07999999999999963</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -5265,7 +5301,7 @@
         <v>384</v>
       </c>
       <c r="B68">
-        <v>0.009999999999999787</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -5281,7 +5317,7 @@
         <v>386</v>
       </c>
       <c r="B70">
-        <v>0.009999999999999898</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -5313,7 +5349,7 @@
         <v>390</v>
       </c>
       <c r="B74">
-        <v>0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -5321,7 +5357,7 @@
         <v>391</v>
       </c>
       <c r="B75">
-        <v>0.01999999999999996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -5329,7 +5365,7 @@
         <v>392</v>
       </c>
       <c r="B76">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -5337,7 +5373,7 @@
         <v>393</v>
       </c>
       <c r="B77">
-        <v>0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -5401,7 +5437,7 @@
         <v>401</v>
       </c>
       <c r="B85">
-        <v>0.1199999999999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -5409,7 +5445,7 @@
         <v>402</v>
       </c>
       <c r="B86">
-        <v>-0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -5425,7 +5461,7 @@
         <v>404</v>
       </c>
       <c r="B88">
-        <v>0.03999999999999992</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -5433,7 +5469,7 @@
         <v>405</v>
       </c>
       <c r="B89">
-        <v>0.02999999999999992</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -5473,7 +5509,7 @@
         <v>410</v>
       </c>
       <c r="B94">
-        <v>-0.2599999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -5481,7 +5517,7 @@
         <v>411</v>
       </c>
       <c r="B95">
-        <v>0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -5561,7 +5597,7 @@
         <v>421</v>
       </c>
       <c r="B105">
-        <v>0.09999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -5585,7 +5621,7 @@
         <v>424</v>
       </c>
       <c r="B108">
-        <v>0.04000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -5601,7 +5637,7 @@
         <v>426</v>
       </c>
       <c r="B110">
-        <v>0.04000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -5609,7 +5645,7 @@
         <v>427</v>
       </c>
       <c r="B111">
-        <v>-0.1199999999999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -5665,7 +5701,7 @@
         <v>434</v>
       </c>
       <c r="B118">
-        <v>0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -5681,7 +5717,7 @@
         <v>436</v>
       </c>
       <c r="B120">
-        <v>0.009999999999999995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -5758,7 +5794,7 @@
         <v>443</v>
       </c>
       <c r="B2">
-        <v>0.01999999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5846,7 +5882,7 @@
         <v>454</v>
       </c>
       <c r="B13">
-        <v>0.2400000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -5870,7 +5906,7 @@
         <v>457</v>
       </c>
       <c r="B16">
-        <v>0.009999999999999995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -5958,7 +5994,7 @@
         <v>468</v>
       </c>
       <c r="B27">
-        <v>-0.04000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -5982,7 +6018,7 @@
         <v>471</v>
       </c>
       <c r="B30">
-        <v>0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -6006,7 +6042,7 @@
         <v>474</v>
       </c>
       <c r="B33">
-        <v>-0.01000000000000023</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -6070,7 +6106,7 @@
         <v>482</v>
       </c>
       <c r="B41">
-        <v>-0.03000000000000025</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -6094,7 +6130,7 @@
         <v>485</v>
       </c>
       <c r="B44">
-        <v>-0.1300000000000003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -6102,7 +6138,7 @@
         <v>486</v>
       </c>
       <c r="B45">
-        <v>0.04999999999999982</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -6118,7 +6154,7 @@
         <v>488</v>
       </c>
       <c r="B47">
-        <v>0.07000000000000073</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -6134,7 +6170,7 @@
         <v>490</v>
       </c>
       <c r="B49">
-        <v>-0.0400000000000027</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -6142,7 +6178,7 @@
         <v>491</v>
       </c>
       <c r="B50">
-        <v>-0.009999999999999995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -6150,7 +6186,7 @@
         <v>492</v>
       </c>
       <c r="B51">
-        <v>0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -6158,7 +6194,7 @@
         <v>493</v>
       </c>
       <c r="B52">
-        <v>-0.1000000000000014</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -6190,7 +6226,7 @@
         <v>497</v>
       </c>
       <c r="B56">
-        <v>-0.009999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -6198,7 +6234,7 @@
         <v>498</v>
       </c>
       <c r="B57">
-        <v>0.06999999999999851</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -6230,7 +6266,7 @@
         <v>502</v>
       </c>
       <c r="B61">
-        <v>0.07999999999999918</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -6238,7 +6274,7 @@
         <v>503</v>
       </c>
       <c r="B62">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -6262,7 +6298,7 @@
         <v>506</v>
       </c>
       <c r="B65">
-        <v>0.02000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -6278,7 +6314,7 @@
         <v>508</v>
       </c>
       <c r="B67">
-        <v>0.009999999999999787</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -6302,7 +6338,7 @@
         <v>511</v>
       </c>
       <c r="B70">
-        <v>0.009999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -6318,7 +6354,7 @@
         <v>513</v>
       </c>
       <c r="B72">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -6334,7 +6370,7 @@
         <v>515</v>
       </c>
       <c r="B74">
-        <v>-0.02000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -6342,7 +6378,7 @@
         <v>516</v>
       </c>
       <c r="B75">
-        <v>-0.01000000000000023</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -6350,7 +6386,7 @@
         <v>517</v>
       </c>
       <c r="B76">
-        <v>0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -6406,7 +6442,7 @@
         <v>524</v>
       </c>
       <c r="B83">
-        <v>-0.01000000000000023</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -6414,7 +6450,7 @@
         <v>525</v>
       </c>
       <c r="B84">
-        <v>-0.009999999999999981</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -6430,7 +6466,7 @@
         <v>527</v>
       </c>
       <c r="B86">
-        <v>0.1000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -6462,7 +6498,7 @@
         <v>531</v>
       </c>
       <c r="B90">
-        <v>-0.009999999999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -6510,7 +6546,7 @@
         <v>537</v>
       </c>
       <c r="B96">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -6563,7 +6599,7 @@
         <v>541</v>
       </c>
       <c r="B2">
-        <v>-0.1399999999999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -6587,7 +6623,7 @@
         <v>544</v>
       </c>
       <c r="B5">
-        <v>-0.009999999999999898</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6595,7 +6631,7 @@
         <v>545</v>
       </c>
       <c r="B6">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -6619,7 +6655,7 @@
         <v>548</v>
       </c>
       <c r="B9">
-        <v>-0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -6627,7 +6663,7 @@
         <v>549</v>
       </c>
       <c r="B10">
-        <v>0.05999999999999994</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -6643,7 +6679,7 @@
         <v>551</v>
       </c>
       <c r="B12">
-        <v>0.240000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -6691,7 +6727,7 @@
         <v>557</v>
       </c>
       <c r="B18">
-        <v>-0.2299999999999986</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -6699,7 +6735,7 @@
         <v>558</v>
       </c>
       <c r="B19">
-        <v>0.01000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -6707,7 +6743,7 @@
         <v>559</v>
       </c>
       <c r="B20">
-        <v>-0.04000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -6715,7 +6751,7 @@
         <v>560</v>
       </c>
       <c r="B21">
-        <v>0.03999999999999981</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -6739,7 +6775,7 @@
         <v>563</v>
       </c>
       <c r="B24">
-        <v>-0.1199999999999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -6755,7 +6791,7 @@
         <v>565</v>
       </c>
       <c r="B26">
-        <v>0.6199999999999992</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -6763,7 +6799,7 @@
         <v>566</v>
       </c>
       <c r="B27">
-        <v>0.06000000000000005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -6771,7 +6807,7 @@
         <v>567</v>
       </c>
       <c r="B28">
-        <v>0.04999999999999893</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -6787,7 +6823,7 @@
         <v>569</v>
       </c>
       <c r="B30">
-        <v>-0.02999999999999936</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -6803,7 +6839,7 @@
         <v>571</v>
       </c>
       <c r="B32">
-        <v>-0.1899999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -6811,7 +6847,7 @@
         <v>572</v>
       </c>
       <c r="B33">
-        <v>0.04999999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -6819,7 +6855,7 @@
         <v>573</v>
       </c>
       <c r="B34">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -6827,7 +6863,7 @@
         <v>574</v>
       </c>
       <c r="B35">
-        <v>-0.4599999999999991</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -6835,7 +6871,7 @@
         <v>575</v>
       </c>
       <c r="B36">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -6843,7 +6879,7 @@
         <v>576</v>
       </c>
       <c r="B37">
-        <v>0.09000000000000002</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated files output and processes
</commit_message>
<xml_diff>
--- a/differences_output.xlsx
+++ b/differences_output.xlsx
@@ -2134,7 +2134,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2142,7 +2142,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2158,7 +2158,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2182,7 +2182,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>-0.02999999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2206,7 +2206,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2214,7 +2214,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>0.01999999999999996</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -2261,9 +2261,6 @@
       <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
@@ -2326,7 +2323,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>-0.23</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -2342,7 +2339,7 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>0.06999999999999984</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -2358,7 +2355,7 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -2374,7 +2371,7 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>-0.04000000000000004</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -2389,9 +2386,6 @@
       <c r="A35" t="s">
         <v>35</v>
       </c>
-      <c r="B35">
-        <v>0</v>
-      </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
@@ -2406,7 +2400,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>-0.0900000000000003</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -2414,16 +2408,13 @@
         <v>38</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>39</v>
       </c>
-      <c r="B39">
-        <v>0</v>
-      </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
@@ -2438,7 +2429,7 @@
         <v>41</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>-0.009999999999999995</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -2446,7 +2437,7 @@
         <v>42</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -2462,7 +2453,7 @@
         <v>44</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -2470,7 +2461,7 @@
         <v>45</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>-0.009999999999999953</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -2485,9 +2476,6 @@
       <c r="A47" t="s">
         <v>47</v>
       </c>
-      <c r="B47">
-        <v>0</v>
-      </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
@@ -2510,7 +2498,7 @@
         <v>50</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>-0.02000000000000002</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -2533,16 +2521,13 @@
       <c r="A53" t="s">
         <v>53</v>
       </c>
-      <c r="B53">
-        <v>0</v>
-      </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
         <v>54</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>-0.009999999999999995</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -2550,7 +2535,7 @@
         <v>55</v>
       </c>
       <c r="B55">
-        <v>0</v>
+        <v>0.0199999999999998</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -2558,7 +2543,7 @@
         <v>56</v>
       </c>
       <c r="B56">
-        <v>0</v>
+        <v>-0.06999999999999984</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -2566,7 +2551,7 @@
         <v>57</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>0.009999999999999998</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -2582,7 +2567,7 @@
         <v>59</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>0.009999999999999981</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -2590,23 +2575,20 @@
         <v>60</v>
       </c>
       <c r="B60">
-        <v>0</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
         <v>61</v>
       </c>
-      <c r="B61">
-        <v>0</v>
-      </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
         <v>62</v>
       </c>
       <c r="B62">
-        <v>0</v>
+        <v>-0.01000000000000001</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -2614,7 +2596,7 @@
         <v>63</v>
       </c>
       <c r="B63">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -2622,7 +2604,7 @@
         <v>64</v>
       </c>
       <c r="B64">
-        <v>0</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -2630,7 +2612,7 @@
         <v>65</v>
       </c>
       <c r="B65">
-        <v>0</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -2645,9 +2627,6 @@
       <c r="A67" t="s">
         <v>67</v>
       </c>
-      <c r="B67">
-        <v>0</v>
-      </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
@@ -2662,23 +2641,20 @@
         <v>69</v>
       </c>
       <c r="B69">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
         <v>70</v>
       </c>
-      <c r="B70">
-        <v>0</v>
-      </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
         <v>71</v>
       </c>
       <c r="B71">
-        <v>0</v>
+        <v>0.009999999999999998</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -2694,23 +2670,20 @@
         <v>73</v>
       </c>
       <c r="B73">
-        <v>0</v>
+        <v>-0.02</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
         <v>74</v>
       </c>
-      <c r="B74">
-        <v>0</v>
-      </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
         <v>75</v>
       </c>
       <c r="B75">
-        <v>0</v>
+        <v>-0.1699999999999999</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -2718,7 +2691,7 @@
         <v>76</v>
       </c>
       <c r="B76">
-        <v>0</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -2734,7 +2707,7 @@
         <v>78</v>
       </c>
       <c r="B78">
-        <v>0</v>
+        <v>-0.01000000000000001</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -2742,7 +2715,7 @@
         <v>79</v>
       </c>
       <c r="B79">
-        <v>0</v>
+        <v>0.009999999999999995</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -2758,7 +2731,7 @@
         <v>81</v>
       </c>
       <c r="B81">
-        <v>0</v>
+        <v>-0.02000000000000002</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -2822,7 +2795,7 @@
         <v>89</v>
       </c>
       <c r="B89">
-        <v>0</v>
+        <v>-0.009999999999999988</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -2837,9 +2810,6 @@
       <c r="A91" t="s">
         <v>91</v>
       </c>
-      <c r="B91">
-        <v>0</v>
-      </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
@@ -2862,7 +2832,7 @@
         <v>94</v>
       </c>
       <c r="B94">
-        <v>0</v>
+        <v>-0.04000000000000004</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -2870,7 +2840,7 @@
         <v>95</v>
       </c>
       <c r="B95">
-        <v>0</v>
+        <v>0.04000000000000001</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -2893,16 +2863,13 @@
       <c r="A98" t="s">
         <v>98</v>
       </c>
-      <c r="B98">
-        <v>0</v>
-      </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
         <v>99</v>
       </c>
       <c r="B99">
-        <v>0</v>
+        <v>0.0199999999999998</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -2926,7 +2893,7 @@
         <v>102</v>
       </c>
       <c r="B102">
-        <v>0</v>
+        <v>0.009999999999999995</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -2957,16 +2924,13 @@
       <c r="A106" t="s">
         <v>106</v>
       </c>
-      <c r="B106">
-        <v>0</v>
-      </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
         <v>107</v>
       </c>
       <c r="B107">
-        <v>0</v>
+        <v>-0.01000000000000006</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -2982,7 +2946,7 @@
         <v>109</v>
       </c>
       <c r="B109">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -3014,7 +2978,7 @@
         <v>113</v>
       </c>
       <c r="B113">
-        <v>0</v>
+        <v>-0.01000000000000001</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -3038,7 +3002,7 @@
         <v>116</v>
       </c>
       <c r="B116">
-        <v>0</v>
+        <v>0.009999999999999981</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -3046,7 +3010,7 @@
         <v>117</v>
       </c>
       <c r="B117">
-        <v>0</v>
+        <v>0.01999999999999999</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -3070,7 +3034,7 @@
         <v>120</v>
       </c>
       <c r="B120">
-        <v>0</v>
+        <v>0.009999999999999787</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -3133,16 +3097,13 @@
       <c r="A128" t="s">
         <v>128</v>
       </c>
-      <c r="B128">
-        <v>0</v>
-      </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
         <v>129</v>
       </c>
       <c r="B129">
-        <v>0</v>
+        <v>-0.02000000000000002</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -3158,7 +3119,7 @@
         <v>131</v>
       </c>
       <c r="B131">
-        <v>0</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -3174,7 +3135,7 @@
         <v>133</v>
       </c>
       <c r="B133">
-        <v>0</v>
+        <v>-0.009999999999999998</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -3190,7 +3151,7 @@
         <v>135</v>
       </c>
       <c r="B135">
-        <v>0</v>
+        <v>0.009999999999999995</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -3205,9 +3166,6 @@
       <c r="A137" t="s">
         <v>137</v>
       </c>
-      <c r="B137">
-        <v>0</v>
-      </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
@@ -3246,7 +3204,7 @@
         <v>142</v>
       </c>
       <c r="B142">
-        <v>0</v>
+        <v>-0.05000000000000004</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -3254,7 +3212,7 @@
         <v>143</v>
       </c>
       <c r="B143">
-        <v>0</v>
+        <v>-0.03999999999999999</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -3270,7 +3228,7 @@
         <v>145</v>
       </c>
       <c r="B145">
-        <v>0</v>
+        <v>-0.1699999999999999</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -3286,7 +3244,7 @@
         <v>147</v>
       </c>
       <c r="B147">
-        <v>0</v>
+        <v>0.05000000000000004</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -3301,16 +3259,13 @@
       <c r="A149" t="s">
         <v>149</v>
       </c>
-      <c r="B149">
-        <v>0</v>
-      </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
         <v>150</v>
       </c>
       <c r="B150">
-        <v>0</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -3326,7 +3281,7 @@
         <v>152</v>
       </c>
       <c r="B152">
-        <v>0</v>
+        <v>0.1099999999999977</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -3374,7 +3329,7 @@
         <v>158</v>
       </c>
       <c r="B158">
-        <v>0</v>
+        <v>0.009999999999999998</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -3382,7 +3337,7 @@
         <v>159</v>
       </c>
       <c r="B159">
-        <v>0</v>
+        <v>0.04999999999999993</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -3390,7 +3345,7 @@
         <v>160</v>
       </c>
       <c r="B160">
-        <v>0</v>
+        <v>0.02000000000000046</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -3398,7 +3353,7 @@
         <v>161</v>
       </c>
       <c r="B161">
-        <v>0</v>
+        <v>-0.02999999999999997</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -3429,16 +3384,13 @@
       <c r="A165" t="s">
         <v>165</v>
       </c>
-      <c r="B165">
-        <v>0</v>
-      </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" t="s">
         <v>166</v>
       </c>
       <c r="B166">
-        <v>0</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -3462,7 +3414,7 @@
         <v>169</v>
       </c>
       <c r="B169">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -3485,9 +3437,6 @@
       <c r="A172" t="s">
         <v>172</v>
       </c>
-      <c r="B172">
-        <v>0</v>
-      </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" t="s">
@@ -3510,23 +3459,20 @@
         <v>175</v>
       </c>
       <c r="B175">
-        <v>0</v>
+        <v>-4.440892098500626E-16</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" t="s">
         <v>176</v>
       </c>
-      <c r="B176">
-        <v>0</v>
-      </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" t="s">
         <v>177</v>
       </c>
       <c r="B177">
-        <v>0</v>
+        <v>0.009999999999999995</v>
       </c>
     </row>
     <row r="178" spans="1:2">
@@ -3558,7 +3504,7 @@
         <v>181</v>
       </c>
       <c r="B181">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -3574,7 +3520,7 @@
         <v>183</v>
       </c>
       <c r="B183">
-        <v>0</v>
+        <v>-0.02</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -3598,7 +3544,7 @@
         <v>186</v>
       </c>
       <c r="B186">
-        <v>0</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="187" spans="1:2">
@@ -3630,7 +3576,7 @@
         <v>190</v>
       </c>
       <c r="B190">
-        <v>0</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="191" spans="1:2">
@@ -3677,16 +3623,13 @@
       <c r="A196" t="s">
         <v>196</v>
       </c>
-      <c r="B196">
-        <v>0</v>
-      </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197" t="s">
         <v>197</v>
       </c>
       <c r="B197">
-        <v>0</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -3718,7 +3661,7 @@
         <v>201</v>
       </c>
       <c r="B201">
-        <v>0</v>
+        <v>0.02000000000000002</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -3750,7 +3693,7 @@
         <v>205</v>
       </c>
       <c r="B205">
-        <v>0</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="206" spans="1:2">
@@ -3782,23 +3725,20 @@
         <v>209</v>
       </c>
       <c r="B209">
-        <v>0</v>
+        <v>0.01999999999999996</v>
       </c>
     </row>
     <row r="210" spans="1:2">
       <c r="A210" t="s">
         <v>210</v>
       </c>
-      <c r="B210">
-        <v>0</v>
-      </c>
     </row>
     <row r="211" spans="1:2">
       <c r="A211" t="s">
         <v>211</v>
       </c>
       <c r="B211">
-        <v>0</v>
+        <v>0.6299999999999999</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -3814,7 +3754,7 @@
         <v>213</v>
       </c>
       <c r="B213">
-        <v>0</v>
+        <v>0.1099999999999999</v>
       </c>
     </row>
     <row r="214" spans="1:2">
@@ -3822,7 +3762,7 @@
         <v>214</v>
       </c>
       <c r="B214">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="215" spans="1:2">
@@ -3830,7 +3770,7 @@
         <v>215</v>
       </c>
       <c r="B215">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="216" spans="1:2">
@@ -3838,23 +3778,20 @@
         <v>216</v>
       </c>
       <c r="B216">
-        <v>0</v>
+        <v>0.03999999999999999</v>
       </c>
     </row>
     <row r="217" spans="1:2">
       <c r="A217" t="s">
         <v>217</v>
       </c>
-      <c r="B217">
-        <v>0</v>
-      </c>
     </row>
     <row r="218" spans="1:2">
       <c r="A218" t="s">
         <v>218</v>
       </c>
       <c r="B218">
-        <v>0</v>
+        <v>0.009999999999999995</v>
       </c>
     </row>
     <row r="219" spans="1:2">
@@ -3870,7 +3807,7 @@
         <v>220</v>
       </c>
       <c r="B220">
-        <v>0</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="221" spans="1:2">
@@ -3878,7 +3815,7 @@
         <v>221</v>
       </c>
       <c r="B221">
-        <v>0</v>
+        <v>-0.4499999999999997</v>
       </c>
     </row>
     <row r="222" spans="1:2">
@@ -3886,7 +3823,7 @@
         <v>222</v>
       </c>
       <c r="B222">
-        <v>0</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="223" spans="1:2">
@@ -3925,9 +3862,6 @@
       <c r="A227" t="s">
         <v>227</v>
       </c>
-      <c r="B227">
-        <v>0</v>
-      </c>
     </row>
     <row r="228" spans="1:2">
       <c r="A228" t="s">
@@ -3942,7 +3876,7 @@
         <v>229</v>
       </c>
       <c r="B229">
-        <v>0</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="230" spans="1:2">
@@ -3950,7 +3884,7 @@
         <v>230</v>
       </c>
       <c r="B230">
-        <v>0</v>
+        <v>0.1199999999999992</v>
       </c>
     </row>
     <row r="231" spans="1:2">
@@ -3958,7 +3892,7 @@
         <v>231</v>
       </c>
       <c r="B231">
-        <v>0</v>
+        <v>-0.009999999999999998</v>
       </c>
     </row>
     <row r="232" spans="1:2">
@@ -3989,16 +3923,13 @@
       <c r="A235" t="s">
         <v>235</v>
       </c>
-      <c r="B235">
-        <v>0</v>
-      </c>
     </row>
     <row r="236" spans="1:2">
       <c r="A236" t="s">
         <v>236</v>
       </c>
       <c r="B236">
-        <v>0</v>
+        <v>0.02000000000000002</v>
       </c>
     </row>
     <row r="237" spans="1:2">
@@ -4051,7 +3982,7 @@
         <v>240</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4067,7 +3998,7 @@
         <v>242</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>0.04999999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4075,7 +4006,7 @@
         <v>243</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>-0.01000000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4147,7 +4078,7 @@
         <v>252</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -4171,7 +4102,7 @@
         <v>255</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>0.009999999999999995</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -4195,7 +4126,7 @@
         <v>258</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>-0.03</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -4219,7 +4150,7 @@
         <v>261</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>-0.0900000000000003</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -4235,7 +4166,7 @@
         <v>263</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>0.07000000000000028</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -4251,7 +4182,7 @@
         <v>265</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>-0.009999999999999787</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -4259,7 +4190,7 @@
         <v>266</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -4275,7 +4206,7 @@
         <v>268</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>-0.02000000000000002</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -4283,7 +4214,7 @@
         <v>269</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>0.009999999999999981</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -4291,7 +4222,7 @@
         <v>270</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>-0.009999999999999787</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -4299,7 +4230,7 @@
         <v>74</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>0.0199999999999998</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -4323,7 +4254,7 @@
         <v>273</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -4331,7 +4262,7 @@
         <v>274</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>-0.1299999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -4339,7 +4270,7 @@
         <v>91</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>0.01999999999999996</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -4347,7 +4278,7 @@
         <v>275</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>-0.1600000000000001</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -4395,7 +4326,7 @@
         <v>281</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>-0.05000000000000004</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -4419,7 +4350,7 @@
         <v>284</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>-0.01999999999999999</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -4435,7 +4366,7 @@
         <v>286</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>-0.09999999999999964</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -4443,7 +4374,7 @@
         <v>152</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>0.05999999999999872</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -4451,7 +4382,7 @@
         <v>287</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -4459,7 +4390,7 @@
         <v>288</v>
       </c>
       <c r="B53">
-        <v>0</v>
+        <v>0.02999999999999997</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -4467,7 +4398,7 @@
         <v>289</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>0.01999999999999996</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -4475,7 +4406,7 @@
         <v>154</v>
       </c>
       <c r="B55">
-        <v>0</v>
+        <v>-0.4300000000000015</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -4523,7 +4454,7 @@
         <v>295</v>
       </c>
       <c r="B61">
-        <v>0</v>
+        <v>0.02000000000000002</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -4539,7 +4470,7 @@
         <v>297</v>
       </c>
       <c r="B63">
-        <v>0</v>
+        <v>-0.02000000000000002</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -4555,7 +4486,7 @@
         <v>299</v>
       </c>
       <c r="B65">
-        <v>0</v>
+        <v>-0.1300000000000003</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -4563,7 +4494,7 @@
         <v>300</v>
       </c>
       <c r="B66">
-        <v>0</v>
+        <v>-0.009999999999999998</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -4571,7 +4502,7 @@
         <v>301</v>
       </c>
       <c r="B67">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -4579,7 +4510,7 @@
         <v>302</v>
       </c>
       <c r="B68">
-        <v>0</v>
+        <v>-0.02999999999999997</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -4603,7 +4534,7 @@
         <v>305</v>
       </c>
       <c r="B71">
-        <v>0</v>
+        <v>0.02000000000000002</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -4635,7 +4566,7 @@
         <v>308</v>
       </c>
       <c r="B75">
-        <v>0</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -4643,7 +4574,7 @@
         <v>309</v>
       </c>
       <c r="B76">
-        <v>0</v>
+        <v>-0.01000000000000001</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -4651,7 +4582,7 @@
         <v>213</v>
       </c>
       <c r="B77">
-        <v>0</v>
+        <v>0.1399999999999997</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -4659,7 +4590,7 @@
         <v>310</v>
       </c>
       <c r="B78">
-        <v>0</v>
+        <v>6.92</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -4691,7 +4622,7 @@
         <v>314</v>
       </c>
       <c r="B82">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -4736,7 +4667,7 @@
         <v>316</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>-0.08000000000000185</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4744,7 +4675,7 @@
         <v>317</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>0.07999999999999829</v>
       </c>
     </row>
   </sheetData>
@@ -4772,9 +4703,6 @@
       <c r="A2" t="s">
         <v>318</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
@@ -4797,7 +4725,7 @@
         <v>321</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>0.04000000000000004</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4821,7 +4749,7 @@
         <v>324</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4829,7 +4757,7 @@
         <v>325</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4845,7 +4773,7 @@
         <v>327</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>-0.1399999999999988</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -4853,7 +4781,7 @@
         <v>328</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>-0.05999999999999961</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -4861,7 +4789,7 @@
         <v>329</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>0.05000000000000071</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -4877,7 +4805,7 @@
         <v>331</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>0.03000000000000003</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -4941,7 +4869,7 @@
         <v>339</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>-0.06</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -4949,7 +4877,7 @@
         <v>340</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>-0.02000000000000002</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -4972,9 +4900,6 @@
       <c r="A27" t="s">
         <v>343</v>
       </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
@@ -5021,7 +4946,7 @@
         <v>349</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -5037,7 +4962,7 @@
         <v>351</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>-0.01000000000000001</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -5045,7 +4970,7 @@
         <v>352</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>-0.01999999999999991</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -5053,7 +4978,7 @@
         <v>353</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>-0.009999999999999898</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -5061,7 +4986,7 @@
         <v>354</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>-0.009999999999999953</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -5109,7 +5034,7 @@
         <v>360</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>0.05000000000000071</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -5117,7 +5042,7 @@
         <v>361</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>0.02000000000000002</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -5141,7 +5066,7 @@
         <v>364</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>-0.009999999999999343</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -5197,7 +5122,7 @@
         <v>371</v>
       </c>
       <c r="B55">
-        <v>0</v>
+        <v>-0.01000000000000001</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -5213,7 +5138,7 @@
         <v>373</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>0.01000000000000068</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -5229,7 +5154,7 @@
         <v>375</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -5237,7 +5162,7 @@
         <v>376</v>
       </c>
       <c r="B60">
-        <v>0</v>
+        <v>0.02000000000000013</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -5245,7 +5170,7 @@
         <v>377</v>
       </c>
       <c r="B61">
-        <v>0</v>
+        <v>0.009999999999999898</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -5253,7 +5178,7 @@
         <v>378</v>
       </c>
       <c r="B62">
-        <v>0</v>
+        <v>0.03999999999999915</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -5261,7 +5186,7 @@
         <v>379</v>
       </c>
       <c r="B63">
-        <v>0</v>
+        <v>-0.01000000000000023</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -5269,7 +5194,7 @@
         <v>380</v>
       </c>
       <c r="B64">
-        <v>0</v>
+        <v>-0.1199999999999992</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -5285,7 +5210,7 @@
         <v>382</v>
       </c>
       <c r="B66">
-        <v>0</v>
+        <v>0.07999999999999963</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -5301,7 +5226,7 @@
         <v>384</v>
       </c>
       <c r="B68">
-        <v>0</v>
+        <v>0.009999999999999787</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -5317,7 +5242,7 @@
         <v>386</v>
       </c>
       <c r="B70">
-        <v>0</v>
+        <v>0.009999999999999898</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -5340,16 +5265,13 @@
       <c r="A73" t="s">
         <v>389</v>
       </c>
-      <c r="B73">
-        <v>0</v>
-      </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
         <v>390</v>
       </c>
       <c r="B74">
-        <v>0</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -5357,7 +5279,7 @@
         <v>391</v>
       </c>
       <c r="B75">
-        <v>0</v>
+        <v>0.01999999999999996</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -5365,7 +5287,7 @@
         <v>392</v>
       </c>
       <c r="B76">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -5373,7 +5295,7 @@
         <v>393</v>
       </c>
       <c r="B77">
-        <v>0</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -5437,7 +5359,7 @@
         <v>401</v>
       </c>
       <c r="B85">
-        <v>0</v>
+        <v>0.1199999999999997</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -5445,7 +5367,7 @@
         <v>402</v>
       </c>
       <c r="B86">
-        <v>0</v>
+        <v>-0.01000000000000001</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -5461,7 +5383,7 @@
         <v>404</v>
       </c>
       <c r="B88">
-        <v>0</v>
+        <v>0.03999999999999992</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -5469,7 +5391,7 @@
         <v>405</v>
       </c>
       <c r="B89">
-        <v>0</v>
+        <v>0.02999999999999992</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -5509,7 +5431,7 @@
         <v>410</v>
       </c>
       <c r="B94">
-        <v>0</v>
+        <v>-0.2599999999999999</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -5517,7 +5439,7 @@
         <v>411</v>
       </c>
       <c r="B95">
-        <v>0</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -5532,9 +5454,6 @@
       <c r="A97" t="s">
         <v>413</v>
       </c>
-      <c r="B97">
-        <v>0</v>
-      </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
@@ -5597,7 +5516,7 @@
         <v>421</v>
       </c>
       <c r="B105">
-        <v>0</v>
+        <v>0.09999999999999998</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -5621,7 +5540,7 @@
         <v>424</v>
       </c>
       <c r="B108">
-        <v>0</v>
+        <v>0.04000000000000004</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -5637,7 +5556,7 @@
         <v>426</v>
       </c>
       <c r="B110">
-        <v>0</v>
+        <v>0.04000000000000001</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -5645,7 +5564,7 @@
         <v>427</v>
       </c>
       <c r="B111">
-        <v>0</v>
+        <v>-0.1199999999999997</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -5701,7 +5620,7 @@
         <v>434</v>
       </c>
       <c r="B118">
-        <v>0</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -5717,7 +5636,7 @@
         <v>436</v>
       </c>
       <c r="B120">
-        <v>0</v>
+        <v>0.009999999999999995</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -5794,7 +5713,7 @@
         <v>443</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>0.01999999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5882,7 +5801,7 @@
         <v>454</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>0.2400000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -5906,7 +5825,7 @@
         <v>457</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>0.009999999999999995</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -5994,7 +5913,7 @@
         <v>468</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>-0.04000000000000004</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -6018,7 +5937,7 @@
         <v>471</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -6042,7 +5961,7 @@
         <v>474</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>-0.01000000000000023</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -6106,7 +6025,7 @@
         <v>482</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>-0.03000000000000025</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -6130,7 +6049,7 @@
         <v>485</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>-0.1300000000000003</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -6138,7 +6057,7 @@
         <v>486</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>0.04999999999999982</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -6154,7 +6073,7 @@
         <v>488</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>0.07000000000000073</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -6170,7 +6089,7 @@
         <v>490</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>-0.0400000000000027</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -6178,7 +6097,7 @@
         <v>491</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>-0.009999999999999995</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -6186,7 +6105,7 @@
         <v>492</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -6194,7 +6113,7 @@
         <v>493</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>-0.1000000000000014</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -6226,7 +6145,7 @@
         <v>497</v>
       </c>
       <c r="B56">
-        <v>0</v>
+        <v>-0.009999999999999998</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -6234,7 +6153,7 @@
         <v>498</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>0.06999999999999851</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -6266,7 +6185,7 @@
         <v>502</v>
       </c>
       <c r="B61">
-        <v>0</v>
+        <v>0.07999999999999918</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -6274,7 +6193,7 @@
         <v>503</v>
       </c>
       <c r="B62">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -6298,7 +6217,7 @@
         <v>506</v>
       </c>
       <c r="B65">
-        <v>0</v>
+        <v>0.02000000000000002</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -6314,7 +6233,7 @@
         <v>508</v>
       </c>
       <c r="B67">
-        <v>0</v>
+        <v>0.009999999999999787</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -6338,7 +6257,7 @@
         <v>511</v>
       </c>
       <c r="B70">
-        <v>0</v>
+        <v>0.009999999999999998</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -6354,7 +6273,7 @@
         <v>513</v>
       </c>
       <c r="B72">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -6370,7 +6289,7 @@
         <v>515</v>
       </c>
       <c r="B74">
-        <v>0</v>
+        <v>-0.02000000000000002</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -6378,7 +6297,7 @@
         <v>516</v>
       </c>
       <c r="B75">
-        <v>0</v>
+        <v>-0.01000000000000023</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -6386,7 +6305,7 @@
         <v>517</v>
       </c>
       <c r="B76">
-        <v>0</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -6442,7 +6361,7 @@
         <v>524</v>
       </c>
       <c r="B83">
-        <v>0</v>
+        <v>-0.01000000000000023</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -6450,7 +6369,7 @@
         <v>525</v>
       </c>
       <c r="B84">
-        <v>0</v>
+        <v>-0.009999999999999981</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -6466,7 +6385,7 @@
         <v>527</v>
       </c>
       <c r="B86">
-        <v>0</v>
+        <v>0.1000000000000001</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -6498,7 +6417,7 @@
         <v>531</v>
       </c>
       <c r="B90">
-        <v>0</v>
+        <v>-0.009999999999999998</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -6546,7 +6465,7 @@
         <v>537</v>
       </c>
       <c r="B96">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -6599,7 +6518,7 @@
         <v>541</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>-0.1399999999999997</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -6623,7 +6542,7 @@
         <v>544</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>-0.009999999999999898</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6631,7 +6550,7 @@
         <v>545</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -6655,7 +6574,7 @@
         <v>548</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -6663,7 +6582,7 @@
         <v>549</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>0.05999999999999994</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -6679,7 +6598,7 @@
         <v>551</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>0.240000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -6727,7 +6646,7 @@
         <v>557</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>-0.2299999999999986</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -6735,7 +6654,7 @@
         <v>558</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>0.01000000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -6743,7 +6662,7 @@
         <v>559</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>-0.04000000000000004</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -6751,7 +6670,7 @@
         <v>560</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>0.03999999999999981</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -6775,7 +6694,7 @@
         <v>563</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>-0.1199999999999997</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -6791,7 +6710,7 @@
         <v>565</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>0.6199999999999992</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -6799,7 +6718,7 @@
         <v>566</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>0.06000000000000005</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -6807,7 +6726,7 @@
         <v>567</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>0.04999999999999893</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -6823,7 +6742,7 @@
         <v>569</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>-0.02999999999999936</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -6839,7 +6758,7 @@
         <v>571</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>-0.1899999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -6847,7 +6766,7 @@
         <v>572</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>0.04999999999999999</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -6855,7 +6774,7 @@
         <v>573</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -6863,7 +6782,7 @@
         <v>574</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>-0.4599999999999991</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -6871,7 +6790,7 @@
         <v>575</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -6879,7 +6798,7 @@
         <v>576</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>0.09000000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>